<commit_message>
Custom Effect definition, new duration sliders
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Documents/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{456611C4-385E-4818-88D8-DF2BB1B9F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6882965-ED3F-46C2-BA62-14715AA5567B}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{456611C4-385E-4818-88D8-DF2BB1B9F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2937CF42-B19C-4C18-9078-361F3D26741B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9669" uniqueCount="3866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9669" uniqueCount="3867">
   <si>
     <t>name</t>
   </si>
@@ -11763,6 +11763,9 @@
   </si>
   <si>
     <t>((characterService.get_Skills(character, '', 'Skill').find(skill =&gt; Skill_Level('Character', skill.name) == 2) &amp;&amp; characterService.get_Skills(character, '', 'Skill').find(skill =&gt; Skill_Level('Character', skill.name) == 4))) || (this.have(character, characterService, charLevel) &amp;&amp; (characterService.get_Skills(character, '', 'Skill').find(skill =&gt; Skill_Level('Character', skill.name) &gt;= 2) &amp;&amp; characterService.get_Skills(character, '', 'Skill').find(skill =&gt; Skill_Level('Character', skill.name) &gt;= 4)))</t>
+  </si>
+  <si>
+    <t>!characterService.get_CompanionAvailable() || this.have(character, characterService, charLevel)</t>
   </si>
 </sst>
 </file>
@@ -21512,10 +21515,10 @@
   <dimension ref="A1:ACN640"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="19" topLeftCell="ACG41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="19" topLeftCell="UE41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="ACL56" sqref="ACL56"/>
+      <selection pane="bottomRight" activeCell="UI56" sqref="UI56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40486,7 +40489,7 @@
         <v>2820</v>
       </c>
       <c r="UI56" s="7" t="s">
-        <v>3344</v>
+        <v>3866</v>
       </c>
       <c r="VB56" s="7" t="s">
         <v>3040</v>

</xml_diff>

<commit_message>
Other Consumables: Bombs; A feat, a spell and a condition
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Documents/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{456611C4-385E-4818-88D8-DF2BB1B9F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2937CF42-B19C-4C18-9078-361F3D26741B}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{456611C4-385E-4818-88D8-DF2BB1B9F5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69223FE7-C84D-415A-8B57-12A891FD79D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9669" uniqueCount="3867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9681" uniqueCount="3871">
   <si>
     <t>name</t>
   </si>
@@ -11766,6 +11766,18 @@
   </si>
   <si>
     <t>!characterService.get_CompanionAvailable() || this.have(character, characterService, charLevel)</t>
+  </si>
+  <si>
+    <t>Inspire Competence</t>
+  </si>
+  <si>
+    <t>You learn the inspire competence composition cantrip, which aids your allies’ skills.</t>
+  </si>
+  <si>
+    <t>e7b357cb-1141-4829-a535-00b851dd0553</t>
+  </si>
+  <si>
+    <t>Feat: Inspire Competence</t>
   </si>
 </sst>
 </file>
@@ -12310,7 +12322,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -21489,22 +21521,22 @@
     <sortCondition ref="C1:AA1"/>
   </sortState>
   <conditionalFormatting sqref="A2:A4 A50 A30 A28 A25 A17 A6">
-    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A67 A63:A64">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A62">
-    <cfRule type="duplicateValues" dxfId="7" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="73"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21512,13 +21544,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:ACN640"/>
+  <dimension ref="A1:ACO640"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="19" topLeftCell="UE41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="19" topLeftCell="ACI260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="UI56" sqref="UI56"/>
+      <selection pane="bottomRight" activeCell="ACO276" sqref="ACO276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21526,11 +21558,11 @@
     <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="551" width="27.42578125" style="1" customWidth="1"/>
     <col min="552" max="554" width="27.28515625" style="1" customWidth="1"/>
-    <col min="555" max="768" width="27.42578125" style="1" customWidth="1"/>
-    <col min="769" max="16384" width="9.140625" style="1"/>
+    <col min="555" max="769" width="27.42578125" style="1" customWidth="1"/>
+    <col min="770" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -23835,8 +23867,11 @@
       <c r="ACN1" s="1" t="s">
         <v>3833</v>
       </c>
-    </row>
-    <row r="2" spans="1:768" x14ac:dyDescent="0.25">
+      <c r="ACO1" s="1" t="s">
+        <v>3867</v>
+      </c>
+    </row>
+    <row r="2" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -26057,8 +26092,11 @@
       <c r="ACN2" s="1" t="s">
         <v>3834</v>
       </c>
-    </row>
-    <row r="3" spans="1:768" x14ac:dyDescent="0.25">
+      <c r="ACO2" s="1" t="s">
+        <v>3868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -26268,7 +26306,7 @@
         <v>3828</v>
       </c>
     </row>
-    <row r="4" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -27401,7 +27439,7 @@
         <v>3820</v>
       </c>
     </row>
-    <row r="5" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -28550,7 +28588,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="6" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -28643,7 +28681,7 @@
       <c r="ACF6"/>
       <c r="ACG6"/>
     </row>
-    <row r="7" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -28730,7 +28768,7 @@
       <c r="ACF7"/>
       <c r="ACG7"/>
     </row>
-    <row r="8" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -29377,7 +29415,7 @@
       <c r="ACF8"/>
       <c r="ACG8"/>
     </row>
-    <row r="9" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -29529,7 +29567,7 @@
       <c r="ACF9"/>
       <c r="ACG9"/>
     </row>
-    <row r="10" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -30149,7 +30187,7 @@
       <c r="ACF10"/>
       <c r="ACG10"/>
     </row>
-    <row r="11" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -30238,7 +30276,7 @@
       <c r="ACF11"/>
       <c r="ACG11"/>
     </row>
-    <row r="12" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -30369,7 +30407,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="13" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -30408,7 +30446,7 @@
       <c r="ZG13"/>
       <c r="ZH13"/>
     </row>
-    <row r="14" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -32629,8 +32667,11 @@
       <c r="ACN14" s="1" t="s">
         <v>3834</v>
       </c>
-    </row>
-    <row r="15" spans="1:768" x14ac:dyDescent="0.25">
+      <c r="ACO14" s="1" t="s">
+        <v>3868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -32781,7 +32822,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="16" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -32789,7 +32830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -32938,7 +32979,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="18" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3835</v>
       </c>
@@ -32946,7 +32987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:768" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:769" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -33005,7 +33046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -34848,8 +34889,11 @@
       <c r="ACN20" s="5" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="21" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO20" s="5" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
@@ -35742,7 +35786,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="22" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
@@ -36011,7 +36055,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="23" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>69</v>
       </c>
@@ -36097,7 +36141,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="24" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
@@ -36132,7 +36176,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="25" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>106</v>
       </c>
@@ -36143,7 +36187,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="26" spans="1:768" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:769" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>563</v>
       </c>
@@ -36151,7 +36195,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="27" spans="1:768" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:769" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
@@ -38018,8 +38062,11 @@
       <c r="ACN27" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:768" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO27" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>95</v>
       </c>
@@ -38060,7 +38107,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="29" spans="1:768" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>96</v>
       </c>
@@ -38101,7 +38148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:768" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2772</v>
       </c>
@@ -38112,7 +38159,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="31" spans="1:768" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>2773</v>
       </c>
@@ -38123,7 +38170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:768" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:769" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
@@ -38618,6 +38665,9 @@
       </c>
       <c r="ACN32" s="3" t="s">
         <v>3806</v>
+      </c>
+      <c r="ACO32" s="3" t="s">
+        <v>2050</v>
       </c>
     </row>
     <row r="33" spans="1:768" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -50726,12 +50776,12 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="257" spans="1:694" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:769" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
         <v>3530</v>
       </c>
     </row>
-    <row r="258" spans="1:694" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:769" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
         <v>215</v>
       </c>
@@ -50739,7 +50789,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="259" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>216</v>
       </c>
@@ -50863,8 +50913,11 @@
       <c r="ZR259" s="2" t="s">
         <v>2140</v>
       </c>
-    </row>
-    <row r="260" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO259" s="2" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="260" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>52</v>
       </c>
@@ -50878,7 +50931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>6</v>
       </c>
@@ -51002,8 +51055,11 @@
       <c r="ZR261" s="2" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="262" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO261" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="262" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>53</v>
       </c>
@@ -51014,7 +51070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>7</v>
       </c>
@@ -51138,8 +51194,11 @@
       <c r="ZR263" s="2" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="264" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO263" s="2" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="264" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>39</v>
       </c>
@@ -51147,7 +51206,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="265" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>3360</v>
       </c>
@@ -51155,7 +51214,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="266" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>3361</v>
       </c>
@@ -51163,7 +51222,7 @@
         <v>3238</v>
       </c>
     </row>
-    <row r="267" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>3362</v>
       </c>
@@ -51171,7 +51230,7 @@
         <v>3239</v>
       </c>
     </row>
-    <row r="268" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>3363</v>
       </c>
@@ -51179,7 +51238,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="269" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>3364</v>
       </c>
@@ -51187,7 +51246,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="270" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>3365</v>
       </c>
@@ -51195,7 +51254,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="271" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>3366</v>
       </c>
@@ -51203,7 +51262,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="272" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>3367</v>
       </c>
@@ -51211,7 +51270,7 @@
         <v>2223</v>
       </c>
     </row>
-    <row r="273" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>40</v>
       </c>
@@ -51222,7 +51281,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="274" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>8</v>
       </c>
@@ -51346,8 +51405,11 @@
       <c r="ZR274" s="2" t="s">
         <v>3593</v>
       </c>
-    </row>
-    <row r="275" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO274" s="2" t="s">
+        <v>3869</v>
+      </c>
+    </row>
+    <row r="275" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>217</v>
       </c>
@@ -51355,7 +51417,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="276" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>9</v>
       </c>
@@ -51473,8 +51535,11 @@
       <c r="ZR276" s="2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="277" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO276" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>10</v>
       </c>
@@ -51598,8 +51663,11 @@
       <c r="ZR277" s="2" t="s">
         <v>3601</v>
       </c>
-    </row>
-    <row r="278" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO277" s="2" t="s">
+        <v>3870</v>
+      </c>
+    </row>
+    <row r="278" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>218</v>
       </c>
@@ -51714,8 +51782,11 @@
       <c r="ZR278" s="2" t="s">
         <v>2141</v>
       </c>
-    </row>
-    <row r="279" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO278" s="2" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="279" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>11</v>
       </c>
@@ -51830,8 +51901,11 @@
       <c r="ZR279" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="280" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO279" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>12</v>
       </c>
@@ -51946,8 +52020,11 @@
       <c r="ZR280" s="2" t="s">
         <v>2223</v>
       </c>
-    </row>
-    <row r="281" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ACO280" s="2" t="s">
+        <v>3867</v>
+      </c>
+    </row>
+    <row r="281" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>219</v>
       </c>
@@ -51955,7 +52032,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="282" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>564</v>
       </c>
@@ -51963,7 +52040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>565</v>
       </c>
@@ -51971,7 +52048,7 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="284" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>566</v>
       </c>
@@ -51979,7 +52056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>567</v>
       </c>
@@ -51987,7 +52064,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="286" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>568</v>
       </c>
@@ -51995,7 +52072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>569</v>
       </c>
@@ -52003,7 +52080,7 @@
         <v>2293</v>
       </c>
     </row>
-    <row r="288" spans="1:694" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:769" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>570</v>
       </c>
@@ -57998,25 +58075,31 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B1:YO1 ZY1:AAA1 ABU1 ABA1 AAY1 AAV1 AAN1 AAC1">
-    <cfRule type="duplicateValues" dxfId="6" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ZK1:ZR1">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:ACG1">
-    <cfRule type="duplicateValues" dxfId="4" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ACK1:ACL1 ACH1:ACI1">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACJ1">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACM1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="ACJ1">
+  <conditionalFormatting sqref="ACN1">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="ACM1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="ACO1">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="ACN1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="ACO1">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some Items Wand functionality changes Orc Ancestry and Badlands Orc Heritage
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="8_{17CD5D8C-B767-4812-956D-A9B96DF27B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E753F328-5EF7-46F7-964D-E8AECBF6D4E7}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="8_{17CD5D8C-B767-4812-956D-A9B96DF27B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C14EB5A-6D15-4F8D-961B-E233390022F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3510" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feats" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11397" uniqueCount="4843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11407" uniqueCount="4849">
   <si>
     <t>name</t>
   </si>
@@ -14708,6 +14708,24 @@
   </si>
   <si>
     <t>You stick to walls with a preternatural grip. You gain a climb Speed of 15 feet.</t>
+  </si>
+  <si>
+    <t>Badlands Orc</t>
+  </si>
+  <si>
+    <t>Badlands Orc Hustle</t>
+  </si>
+  <si>
+    <t>You can Hustle twice as long while exploring before you have to stop.</t>
+  </si>
+  <si>
+    <t>You come from sun-scorched badlands, where long legs and an ability to withstand the elements helped you thrive. You can Hustle twice as long while exploring before you have to stop.</t>
+  </si>
+  <si>
+    <t>You come from sun-scorched badlands, where long legs and an ability to withstand the elements helped you thrive.</t>
+  </si>
+  <si>
+    <t>You come from sun-scorched badlands, where long legs and an ability to withstand the elements helped you thrive. You treat environmental heat effects as if they were one step less extreme (incredible heat becomes extreme, extreme heat becomes severe, and so on).</t>
   </si>
 </sst>
 </file>
@@ -15197,7 +15215,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyAlignment="1"/>
@@ -15208,9 +15226,6 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="39" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="35" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15749,14 +15764,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AKC949"/>
+  <dimension ref="A1:AKE949"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="19" topLeftCell="AJC53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="19" topLeftCell="AJW20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="PE338" sqref="PE338"/>
       <selection pane="topRight" activeCell="PE338" sqref="PE338"/>
       <selection pane="bottomLeft" activeCell="PE338" sqref="PE338"/>
-      <selection pane="bottomRight" activeCell="AJG56" sqref="AJG56"/>
+      <selection pane="bottomRight" activeCell="AKD1" sqref="AKD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15764,11 +15779,11 @@
     <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="539" width="27.42578125" style="1" customWidth="1"/>
     <col min="540" max="542" width="27.28515625" style="1" customWidth="1"/>
-    <col min="543" max="965" width="27.42578125" style="1" customWidth="1"/>
-    <col min="966" max="16384" width="9.140625" style="1"/>
+    <col min="543" max="967" width="27.42578125" style="1" customWidth="1"/>
+    <col min="968" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18664,8 +18679,14 @@
       <c r="AKC1" s="1" t="s">
         <v>4740</v>
       </c>
-    </row>
-    <row r="2" spans="1:965" x14ac:dyDescent="0.25">
+      <c r="AKD1" s="1" t="s">
+        <v>4843</v>
+      </c>
+      <c r="AKE1" s="1" t="s">
+        <v>4844</v>
+      </c>
+    </row>
+    <row r="2" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -18858,7 +18879,7 @@
       <c r="BL2" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="BM2" s="10" t="s">
+      <c r="BM2" s="1" t="s">
         <v>821</v>
       </c>
       <c r="BN2" s="1" t="s">
@@ -18897,7 +18918,7 @@
       <c r="BY2" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="BZ2" s="10" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>875</v>
       </c>
       <c r="CA2" s="1" t="s">
@@ -19032,7 +19053,7 @@
       <c r="DR2" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="DS2" s="10" t="s">
+      <c r="DS2" s="1" t="s">
         <v>1070</v>
       </c>
       <c r="DT2" s="1" t="s">
@@ -19041,7 +19062,7 @@
       <c r="DU2" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="DV2" s="10" t="s">
+      <c r="DV2" s="1" t="s">
         <v>4817</v>
       </c>
       <c r="DW2" s="1" t="s">
@@ -19218,7 +19239,7 @@
       <c r="GB2" s="1" t="s">
         <v>1337</v>
       </c>
-      <c r="GC2" s="10" t="s">
+      <c r="GC2" s="1" t="s">
         <v>2304</v>
       </c>
       <c r="GD2" s="1" t="s">
@@ -19311,7 +19332,7 @@
       <c r="HG2" s="1" t="s">
         <v>1453</v>
       </c>
-      <c r="HH2" s="10" t="s">
+      <c r="HH2" s="1" t="s">
         <v>4818</v>
       </c>
       <c r="HI2" s="1" t="s">
@@ -19335,7 +19356,7 @@
       <c r="HO2" s="1" t="s">
         <v>1482</v>
       </c>
-      <c r="HP2" s="10" t="s">
+      <c r="HP2" s="1" t="s">
         <v>4819</v>
       </c>
       <c r="HQ2" s="1" t="s">
@@ -19368,7 +19389,7 @@
       <c r="HZ2" s="1" t="s">
         <v>1517</v>
       </c>
-      <c r="IA2" s="10" t="s">
+      <c r="IA2" s="1" t="s">
         <v>1520</v>
       </c>
       <c r="IB2" s="1" t="s">
@@ -19401,7 +19422,7 @@
       <c r="IK2" s="1" t="s">
         <v>1553</v>
       </c>
-      <c r="IL2" s="10" t="s">
+      <c r="IL2" s="1" t="s">
         <v>2729</v>
       </c>
       <c r="IM2" s="1" t="s">
@@ -19620,7 +19641,7 @@
       <c r="LF2" s="1" t="s">
         <v>1844</v>
       </c>
-      <c r="LG2" s="10" t="s">
+      <c r="LG2" s="1" t="s">
         <v>4823</v>
       </c>
       <c r="LH2" s="1" t="s">
@@ -19863,7 +19884,7 @@
       <c r="OZ2" s="1" t="s">
         <v>2699</v>
       </c>
-      <c r="PF2" s="10" t="s">
+      <c r="PF2" s="1" t="s">
         <v>2286</v>
       </c>
       <c r="PG2" s="1" t="s">
@@ -19884,7 +19905,7 @@
       <c r="PP2" s="1" t="s">
         <v>2237</v>
       </c>
-      <c r="PQ2" s="10" t="s">
+      <c r="PQ2" s="1" t="s">
         <v>2296</v>
       </c>
       <c r="PR2" s="1" t="s">
@@ -20079,7 +20100,7 @@
       <c r="SC2" s="1" t="s">
         <v>3076</v>
       </c>
-      <c r="SD2" s="10" t="s">
+      <c r="SD2" s="1" t="s">
         <v>3077</v>
       </c>
       <c r="SE2" s="1" t="s">
@@ -20214,7 +20235,7 @@
       <c r="TV2" s="1" t="s">
         <v>2795</v>
       </c>
-      <c r="TW2" s="10" t="s">
+      <c r="TW2" s="1" t="s">
         <v>653</v>
       </c>
       <c r="TX2" s="1" t="s">
@@ -20229,7 +20250,7 @@
       <c r="UA2" s="1" t="s">
         <v>2802</v>
       </c>
-      <c r="UB2" s="10" t="s">
+      <c r="UB2" s="1" t="s">
         <v>3092</v>
       </c>
       <c r="UC2" s="1" t="s">
@@ -20280,25 +20301,25 @@
       <c r="UR2" s="1" t="s">
         <v>3096</v>
       </c>
-      <c r="US2" s="10" t="s">
+      <c r="US2" s="1" t="s">
         <v>3097</v>
       </c>
-      <c r="UT2" s="10" t="s">
+      <c r="UT2" s="1" t="s">
         <v>3098</v>
       </c>
-      <c r="UU2" s="10" t="s">
+      <c r="UU2" s="1" t="s">
         <v>3099</v>
       </c>
-      <c r="UV2" s="10" t="s">
+      <c r="UV2" s="1" t="s">
         <v>3100</v>
       </c>
-      <c r="UW2" s="10" t="s">
+      <c r="UW2" s="1" t="s">
         <v>3101</v>
       </c>
       <c r="UX2" s="1" t="s">
         <v>2824</v>
       </c>
-      <c r="UY2" s="10" t="s">
+      <c r="UY2" s="1" t="s">
         <v>3102</v>
       </c>
       <c r="UZ2" s="1" t="s">
@@ -20310,7 +20331,7 @@
       <c r="VB2" s="1" t="s">
         <v>3104</v>
       </c>
-      <c r="VC2" s="10" t="s">
+      <c r="VC2" s="1" t="s">
         <v>3105</v>
       </c>
       <c r="VD2" s="1" t="s">
@@ -20598,7 +20619,7 @@
       <c r="YT2" s="1" t="s">
         <v>3497</v>
       </c>
-      <c r="YU2" s="10" t="s">
+      <c r="YU2" s="1" t="s">
         <v>3582</v>
       </c>
       <c r="YV2" s="1" t="s">
@@ -20652,19 +20673,19 @@
       <c r="ZL2" s="1" t="s">
         <v>3538</v>
       </c>
-      <c r="ZM2" s="10" t="s">
+      <c r="ZM2" s="1" t="s">
         <v>3894</v>
       </c>
-      <c r="ZN2" s="10" t="s">
+      <c r="ZN2" s="1" t="s">
         <v>3895</v>
       </c>
-      <c r="ZO2" s="10" t="s">
+      <c r="ZO2" s="1" t="s">
         <v>2285</v>
       </c>
       <c r="ZP2" s="1" t="s">
         <v>3588</v>
       </c>
-      <c r="ZQ2" s="10" t="s">
+      <c r="ZQ2" s="1" t="s">
         <v>2290</v>
       </c>
       <c r="ZR2" s="1" t="s">
@@ -20736,7 +20757,7 @@
       <c r="AAN2" s="1" t="s">
         <v>3611</v>
       </c>
-      <c r="AAO2" s="10" t="s">
+      <c r="AAO2" s="1" t="s">
         <v>2439</v>
       </c>
       <c r="AAP2" s="1" t="s">
@@ -20763,7 +20784,7 @@
       <c r="AAW2" s="1" t="s">
         <v>3695</v>
       </c>
-      <c r="AAX2" s="10" t="s">
+      <c r="AAX2" s="1" t="s">
         <v>3912</v>
       </c>
       <c r="AAY2" s="1" t="s">
@@ -20877,7 +20898,7 @@
       <c r="ACI2" s="1" t="s">
         <v>3859</v>
       </c>
-      <c r="ACJ2" s="10" t="s">
+      <c r="ACJ2" s="1" t="s">
         <v>3921</v>
       </c>
       <c r="ACK2" s="1" t="s">
@@ -20958,7 +20979,7 @@
       <c r="ADJ2" s="1" t="s">
         <v>3999</v>
       </c>
-      <c r="ADK2" s="10" t="s">
+      <c r="ADK2" s="1" t="s">
         <v>4797</v>
       </c>
       <c r="ADL2" s="1" t="s">
@@ -20976,7 +20997,7 @@
       <c r="ADP2" s="1" t="s">
         <v>4798</v>
       </c>
-      <c r="ADQ2" s="10" t="s">
+      <c r="ADQ2" s="1" t="s">
         <v>4799</v>
       </c>
       <c r="ADR2" s="1" t="s">
@@ -21018,7 +21039,7 @@
       <c r="AFR2" s="1" t="s">
         <v>4837</v>
       </c>
-      <c r="AGB2" s="10" t="s">
+      <c r="AGB2" s="1" t="s">
         <v>4801</v>
       </c>
       <c r="AGC2" s="1" t="s">
@@ -21114,8 +21135,14 @@
       <c r="AKC2" s="1" t="s">
         <v>4742</v>
       </c>
-    </row>
-    <row r="3" spans="1:965" x14ac:dyDescent="0.25">
+      <c r="AKD2" s="1" t="s">
+        <v>4848</v>
+      </c>
+      <c r="AKE2" s="1" t="s">
+        <v>4846</v>
+      </c>
+    </row>
+    <row r="3" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -21270,7 +21297,7 @@
         <v>4810</v>
       </c>
     </row>
-    <row r="4" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -21412,7 +21439,7 @@
       <c r="BL4" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="BM4" s="10" t="s">
+      <c r="BM4" s="1" t="s">
         <v>823</v>
       </c>
       <c r="BO4" s="1" t="s">
@@ -21445,7 +21472,7 @@
       <c r="BY4" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="BZ4" s="10" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>876</v>
       </c>
       <c r="CA4" s="1" t="s">
@@ -21487,7 +21514,7 @@
       <c r="CP4" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="CQ4" s="10" t="s">
+      <c r="CQ4" s="1" t="s">
         <v>942</v>
       </c>
       <c r="CS4" s="1" t="s">
@@ -21745,7 +21772,7 @@
       <c r="HG4" s="1" t="s">
         <v>1457</v>
       </c>
-      <c r="HH4" s="10" t="s">
+      <c r="HH4" s="1" t="s">
         <v>4818</v>
       </c>
       <c r="HK4" s="1" t="s">
@@ -21958,7 +21985,7 @@
       <c r="LF4" s="1" t="s">
         <v>1846</v>
       </c>
-      <c r="LG4" s="10" t="s">
+      <c r="LG4" s="1" t="s">
         <v>4821</v>
       </c>
       <c r="LI4" s="1" t="s">
@@ -22069,7 +22096,7 @@
       <c r="RZ4" s="1" t="s">
         <v>2535</v>
       </c>
-      <c r="SD4" s="10" t="s">
+      <c r="SD4" s="1" t="s">
         <v>3126</v>
       </c>
       <c r="SE4" s="1" t="s">
@@ -22150,16 +22177,16 @@
       <c r="UR4" s="1" t="s">
         <v>3134</v>
       </c>
-      <c r="UT4" s="10" t="s">
+      <c r="UT4" s="1" t="s">
         <v>3135</v>
       </c>
-      <c r="UU4" s="10" t="s">
+      <c r="UU4" s="1" t="s">
         <v>3136</v>
       </c>
-      <c r="UV4" s="10" t="s">
+      <c r="UV4" s="1" t="s">
         <v>3137</v>
       </c>
-      <c r="UW4" s="10" t="s">
+      <c r="UW4" s="1" t="s">
         <v>3138</v>
       </c>
       <c r="UY4" s="1" t="s">
@@ -22174,7 +22201,7 @@
       <c r="VB4" s="1" t="s">
         <v>3141</v>
       </c>
-      <c r="VC4" s="10" t="s">
+      <c r="VC4" s="1" t="s">
         <v>3142</v>
       </c>
       <c r="VE4" s="1" t="s">
@@ -22303,7 +22330,7 @@
       <c r="YT4" s="1" t="s">
         <v>3366</v>
       </c>
-      <c r="YU4" s="10" t="s">
+      <c r="YU4" s="1" t="s">
         <v>3583</v>
       </c>
       <c r="YV4" s="1" t="s">
@@ -22318,7 +22345,7 @@
       <c r="ZO4" s="1" t="s">
         <v>2081</v>
       </c>
-      <c r="ZQ4" s="10" t="s">
+      <c r="ZQ4" s="1" t="s">
         <v>2291</v>
       </c>
       <c r="ZT4" s="1" t="s">
@@ -22345,7 +22372,7 @@
       <c r="AAL4" s="1" t="s">
         <v>3689</v>
       </c>
-      <c r="AAO4" s="10" t="s">
+      <c r="AAO4" s="1" t="s">
         <v>2302</v>
       </c>
       <c r="AAQ4" s="1" t="s">
@@ -22363,7 +22390,7 @@
       <c r="AAW4" s="1" t="s">
         <v>3696</v>
       </c>
-      <c r="AAX4" s="10" t="s">
+      <c r="AAX4" s="1" t="s">
         <v>3933</v>
       </c>
       <c r="AAY4" s="1" t="s">
@@ -22417,7 +22444,7 @@
       <c r="ADJ4" s="1" t="s">
         <v>4000</v>
       </c>
-      <c r="ADK4" s="10" t="s">
+      <c r="ADK4" s="1" t="s">
         <v>4812</v>
       </c>
       <c r="ADP4" s="1" t="s">
@@ -22471,8 +22498,14 @@
       <c r="AKC4" s="1" t="s">
         <v>4743</v>
       </c>
-    </row>
-    <row r="5" spans="1:965" x14ac:dyDescent="0.25">
+      <c r="AKD4" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="AKE4" s="1" t="s">
+        <v>4845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -23646,8 +23679,14 @@
       <c r="AKC5" s="1" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="6" spans="1:965" x14ac:dyDescent="0.25">
+      <c r="AKD5" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="AKE5" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -23661,7 +23700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>90</v>
       </c>
@@ -23714,7 +23753,7 @@
         <v>4304</v>
       </c>
     </row>
-    <row r="8" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -24340,7 +24379,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="9" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -24426,7 +24465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -25025,7 +25064,7 @@
         <v>4364</v>
       </c>
     </row>
-    <row r="11" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>121</v>
       </c>
@@ -25048,7 +25087,7 @@
         <v>3977</v>
       </c>
     </row>
-    <row r="12" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -25191,7 +25230,7 @@
         <v>4815</v>
       </c>
     </row>
-    <row r="13" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -25202,7 +25241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -28020,8 +28059,14 @@
       <c r="AKC14" s="1" t="s">
         <v>4741</v>
       </c>
-    </row>
-    <row r="15" spans="1:965" x14ac:dyDescent="0.25">
+      <c r="AKD14" s="1" t="s">
+        <v>4847</v>
+      </c>
+      <c r="AKE14" s="1" t="s">
+        <v>4847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
@@ -28224,7 +28269,7 @@
         <v>2456</v>
       </c>
     </row>
-    <row r="16" spans="1:965" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:967" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Custom feats and items Custom Kitsune ancestry, heritages and feats
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="381" documentId="8_{17CD5D8C-B767-4812-956D-A9B96DF27B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8F39E57-15B8-485C-B081-F80414D2C6D3}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="8_{17CD5D8C-B767-4812-956D-A9B96DF27B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7A77AF61-3E6F-42BF-982C-E67563DAB8D4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11401" uniqueCount="4843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11402" uniqueCount="4843">
   <si>
     <t>name</t>
   </si>
@@ -15749,11 +15749,11 @@
   <dimension ref="A1:AKE949"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="19" topLeftCell="XY284" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="19" topLeftCell="DY56" activePane="bottomRight" state="frozen"/>
       <selection activeCell="PE338" sqref="PE338"/>
       <selection pane="topRight" activeCell="PE338" sqref="PE338"/>
       <selection pane="bottomLeft" activeCell="PE338" sqref="PE338"/>
-      <selection pane="bottomRight" activeCell="YC295" sqref="YC295"/>
+      <selection pane="bottomRight" activeCell="EF67" sqref="EF67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38338,8 +38338,8 @@
       <c r="EE67" s="2">
         <v>2</v>
       </c>
-      <c r="EF67" s="2" t="e">
-        <v>#NAME?</v>
+      <c r="EF67" s="2" t="s">
+        <v>1760</v>
       </c>
       <c r="EM67" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
Some items Bugfixes Improvements to cooldowns
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="114_{FA74D905-5457-484E-846B-22923D609547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D5A521F-DFB6-4A14-AD16-1294F4F972A1}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="114_{FA74D905-5457-484E-846B-22923D609547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89AA7DCD-3920-480A-86C3-38C552E22794}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12490" uniqueCount="5206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12490" uniqueCount="5208">
   <si>
     <t>name</t>
   </si>
@@ -16031,6 +16031,12 @@
   </si>
   <si>
     <t>You can use Retributive Strike with a ranged weapon.</t>
+  </si>
+  <si>
+    <t>You can help your whole group get into position. When you use Liberating Step, if your ally doesn't attempt to break free of an effect, you and all allies within 15 feet can Step, in addition to the triggering ally.</t>
+  </si>
+  <si>
+    <t>When you use Liberating Step, if your ally doesn't attempt to break free of an effect, you and all allies within 15 feet can Step, in addition to the triggering ally.</t>
   </si>
 </sst>
 </file>
@@ -20056,20 +20062,17 @@
   <dimension ref="A1:ANU986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="19" topLeftCell="ANN20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="19" topLeftCell="PU20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="PE338" sqref="PE338"/>
       <selection pane="topRight" activeCell="PE338" sqref="PE338"/>
       <selection pane="bottomLeft" activeCell="PE338" sqref="PE338"/>
-      <selection pane="bottomRight" activeCell="ANU2" sqref="ANU2"/>
+      <selection pane="bottomRight" activeCell="PY4" sqref="PY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="625" width="27.42578125" style="1" customWidth="1"/>
-    <col min="626" max="628" width="27.28515625" style="1" customWidth="1"/>
-    <col min="629" max="1060" width="27.42578125" style="1" customWidth="1"/>
-    <col min="1061" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1061" width="27.42578125" style="1" customWidth="1"/>
+    <col min="1062" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1061" customFormat="1" x14ac:dyDescent="0.25">
@@ -24570,7 +24573,7 @@
         <v>5100</v>
       </c>
       <c r="PY2" s="1" t="s">
-        <v>5103</v>
+        <v>5206</v>
       </c>
       <c r="PZ2" s="1" t="s">
         <v>5197</v>
@@ -27025,7 +27028,7 @@
         <v>5101</v>
       </c>
       <c r="PY4" s="1" t="s">
-        <v>5104</v>
+        <v>5207</v>
       </c>
       <c r="QA4" s="1" t="s">
         <v>5115</v>

</xml_diff>

<commit_message>
Some feats Divine Font improvements Anathema in Classes Improved language list updating
</commit_message>
<xml_diff>
--- a/feats.xlsx
+++ b/feats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1397" documentId="6_{DC6D762A-4C8E-421B-B277-4FA25E6B0353}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFEC715F-45D5-4C9E-AB5D-AB9013A3D9BE}"/>
+  <xr:revisionPtr revIDLastSave="1423" documentId="6_{DC6D762A-4C8E-421B-B277-4FA25E6B0353}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C30A591D-D243-46F0-AC77-5CA1C17FF398}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feats" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13562" uniqueCount="5486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13571" uniqueCount="5492">
   <si>
     <t>name</t>
   </si>
@@ -16841,9 +16841,6 @@
     <t>You can use Halfling Luck once per hour, rather than once per day. If you have Guiding Luck, you can still use Halfling Luck when you fail a Perception check or attack roll only once per day (though you can use it within the same hour that you used Halfling Luck), and if you have Shared Luck, you can still use Halfling Luck on an ally instead of yourself only once per day.</t>
   </si>
   <si>
-    <t>character.get_FeatsTaken(0,charLevel).filter(gain =&gt; characterService.get_FeatsAndFeatures(gain.name).some(feat =&gt; feat.traits.includes(\"Stance\"))).length &gt;= 2</t>
-  </si>
-  <si>
     <t>Companion:Stealth Proficiency Level</t>
   </si>
   <si>
@@ -16881,6 +16878,27 @@
   </si>
   <si>
     <t>Storm order</t>
+  </si>
+  <si>
+    <t>character.get_FeatsTaken(0,charLevel).filter(gain =&gt; characterService.get_FeatsAndFeatures(gain.name).some(feat =&gt; feat.traits.includes(\"Stance\"))).length &gt;= 2</t>
+  </si>
+  <si>
+    <t>You carry the fury of the storm within you, channeling it to terrifying effect and riding the winds through the sky. You are trained in Acrobatics. You also gain the Storm Born druid feat. You gain the tempest surge order spell, and you increase the number of Focus Points in your focus pool by 1. Polluting the air or allowing those who cause major air pollution or climate shifts to go unpunished is anathema to your order. (This doesn't force you to take action against merely potential harm to the environment or to sacrifice yourself against an obviously superior foe.)</t>
+  </si>
+  <si>
+    <t>Polluting the air or allowing those who cause major air pollution or climate shifts to go unpunished is anathema to your order. (This doesn't force you to take action against merely potential harm to the environment or to sacrifice yourself against an obviously superior foe.)</t>
+  </si>
+  <si>
+    <t>Character.class.name == 'Druid' ? 1 : 0</t>
+  </si>
+  <si>
+    <t>Feat: Otherworldly Magic</t>
+  </si>
+  <si>
+    <t>Your elven magic manifests as a simple arcane spell, even if you aren't formally trained in magic. Choose one cantrip from the arcane spell list. You can cast this cantrip as an arcane innate spell at will. A cantrip is heightened to a spell level equal to half your level rounded up.</t>
+  </si>
+  <si>
+    <t>cfe25e1d-3c21-4812-b815-5099c0bf4ce0</t>
   </si>
 </sst>
 </file>
@@ -18204,7 +18222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:NP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19358,7 +19376,7 @@
         <v>1867</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5475</v>
+        <v>5474</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="5"/>
@@ -19396,7 +19414,7 @@
       <c r="AK2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AU2" s="1" t="s">
-        <v>5481</v>
+        <v>5480</v>
       </c>
       <c r="BA2" s="5"/>
       <c r="BB2" s="5"/>
@@ -19471,7 +19489,7 @@
       <c r="DK2" s="4"/>
       <c r="DL2" s="4"/>
       <c r="DM2" s="6" t="s">
-        <v>5477</v>
+        <v>5476</v>
       </c>
       <c r="DN2" s="6"/>
       <c r="DO2" s="6"/>
@@ -19554,7 +19572,7 @@
         <v>1</v>
       </c>
       <c r="GL2" s="4" t="s">
-        <v>5476</v>
+        <v>5475</v>
       </c>
       <c r="GM2" s="4"/>
       <c r="GN2" s="4"/>
@@ -19762,7 +19780,7 @@
       <c r="NF2" s="2"/>
       <c r="NG2" s="2"/>
       <c r="NH2" s="2" t="s">
-        <v>5478</v>
+        <v>5477</v>
       </c>
       <c r="NI2" s="2" t="s">
         <v>2059</v>
@@ -19782,21 +19800,21 @@
         <v>1</v>
       </c>
       <c r="NP2" s="2" t="s">
-        <v>5479</v>
+        <v>5478</v>
       </c>
     </row>
     <row r="3" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5476</v>
+        <v>5475</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5482</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>5481</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>5483</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>5482</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>5484</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -19832,7 +19850,7 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AU3" s="1" t="s">
-        <v>5480</v>
+        <v>5479</v>
       </c>
       <c r="BA3" s="5" t="s">
         <v>2059</v>
@@ -19851,7 +19869,7 @@
       <c r="BK3" s="2"/>
       <c r="BL3" s="2"/>
       <c r="BM3" s="3" t="s">
-        <v>5485</v>
+        <v>5484</v>
       </c>
       <c r="BN3" s="3"/>
       <c r="BO3" s="3"/>
@@ -20171,7 +20189,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="0" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="127"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20181,11 +20199,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AOR999"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="QI365" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="ABG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:QJ380"/>
+      <selection pane="bottomRight" activeCell="ABK2" sqref="ABK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21550,7 +21568,7 @@
         <v>1867</v>
       </c>
       <c r="QJ1" t="s">
-        <v>5476</v>
+        <v>5475</v>
       </c>
       <c r="QK1" t="s">
         <v>1868</v>
@@ -24780,10 +24798,10 @@
         <v>4916</v>
       </c>
       <c r="QI2" s="1" t="s">
-        <v>5475</v>
+        <v>5486</v>
       </c>
       <c r="QJ2" s="1" t="s">
-        <v>5483</v>
+        <v>5482</v>
       </c>
       <c r="QL2" s="1" t="s">
         <v>1871</v>
@@ -26482,6 +26500,9 @@
       </c>
       <c r="AMR2" s="1" t="s">
         <v>1263</v>
+      </c>
+      <c r="AMS2" s="1" t="s">
+        <v>5490</v>
       </c>
       <c r="ANM2" s="1" t="s">
         <v>2066</v>
@@ -27349,7 +27370,7 @@
         <v>4863</v>
       </c>
       <c r="QJ4" s="12" t="s">
-        <v>5482</v>
+        <v>5481</v>
       </c>
       <c r="RZ4" s="12" t="s">
         <v>5104</v>
@@ -27851,6 +27872,9 @@
       </c>
       <c r="AJJ4" s="12" t="s">
         <v>5471</v>
+      </c>
+      <c r="AJK4" s="12" t="s">
+        <v>4499</v>
       </c>
       <c r="AJT4" s="12" t="s">
         <v>4448</v>
@@ -28764,7 +28788,7 @@
         <v>4923</v>
       </c>
       <c r="QJ5" s="5" t="s">
-        <v>5484</v>
+        <v>5483</v>
       </c>
       <c r="RZ5" s="5" t="s">
         <v>5429</v>
@@ -34245,10 +34269,10 @@
         <v>4929</v>
       </c>
       <c r="QI47" s="1" t="s">
-        <v>5481</v>
+        <v>5480</v>
       </c>
       <c r="QJ47" s="1" t="s">
-        <v>5480</v>
+        <v>5479</v>
       </c>
       <c r="QL47" s="1" t="s">
         <v>1870</v>
@@ -43746,7 +43770,7 @@
         <v>1862</v>
       </c>
       <c r="QJ65" s="3" t="s">
-        <v>5485</v>
+        <v>5484</v>
       </c>
       <c r="SL65" s="3" t="s">
         <v>2104</v>
@@ -46190,7 +46214,7 @@
         <v>2275</v>
       </c>
       <c r="DX90" s="7" t="s">
-        <v>5472</v>
+        <v>5485</v>
       </c>
       <c r="DZ90" s="7" t="s">
         <v>2270</v>
@@ -46955,7 +46979,7 @@
         <v>1545</v>
       </c>
       <c r="KG93" s="2" t="s">
-        <v>1421</v>
+        <v>1246</v>
       </c>
       <c r="KH93" s="2" t="s">
         <v>1663</v>
@@ -47009,7 +47033,7 @@
         <v>976</v>
       </c>
       <c r="YP93" s="2" t="s">
-        <v>5473</v>
+        <v>5472</v>
       </c>
       <c r="ZE93" s="2" t="s">
         <v>767</v>
@@ -47350,7 +47374,7 @@
         <v>5119</v>
       </c>
       <c r="QI97" s="2" t="s">
-        <v>5119</v>
+        <v>5488</v>
       </c>
       <c r="SK97" s="2">
         <v>1</v>
@@ -47365,7 +47389,7 @@
         <v>5176</v>
       </c>
       <c r="YP97" s="2" t="s">
-        <v>5474</v>
+        <v>5473</v>
       </c>
       <c r="ZE97" s="2">
         <v>2</v>
@@ -47732,7 +47756,7 @@
         <v>5119</v>
       </c>
       <c r="QI102" s="3" t="s">
-        <v>5119</v>
+        <v>5488</v>
       </c>
       <c r="SK102" s="3">
         <v>1</v>
@@ -48017,7 +48041,7 @@
         <v>4781</v>
       </c>
       <c r="QI117" s="6" t="s">
-        <v>5477</v>
+        <v>5487</v>
       </c>
     </row>
     <row r="118" spans="1:1005 1071:1071" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -50377,7 +50401,7 @@
         <v>4835</v>
       </c>
       <c r="QI194" s="4" t="s">
-        <v>5476</v>
+        <v>5475</v>
       </c>
       <c r="WG194" s="4" t="s">
         <v>2580</v>
@@ -60864,7 +60888,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="353" spans="1:1027" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1033" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="7" t="s">
         <v>204</v>
       </c>
@@ -60875,12 +60899,12 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="354" spans="1:1027" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1033" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="7" t="s">
         <v>3268</v>
       </c>
     </row>
-    <row r="355" spans="1:1027" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1033" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="7" t="s">
         <v>205</v>
       </c>
@@ -60891,7 +60915,7 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="356" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>206</v>
       </c>
@@ -61209,8 +61233,11 @@
       <c r="AMM356" s="2" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="357" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS356" s="2" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>49</v>
       </c>
@@ -61277,8 +61304,11 @@
       <c r="AMA357" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="358" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS357" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>6</v>
       </c>
@@ -61584,8 +61614,11 @@
       <c r="AMM358" s="2" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="359" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS358" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>50</v>
       </c>
@@ -61605,7 +61638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>7</v>
       </c>
@@ -61911,8 +61944,11 @@
       <c r="AMM360" s="2" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="361" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS360" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>4602</v>
       </c>
@@ -61989,7 +62025,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="362" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>36</v>
       </c>
@@ -62000,7 +62036,7 @@
         <v>5337</v>
       </c>
     </row>
-    <row r="363" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>3102</v>
       </c>
@@ -62008,7 +62044,7 @@
         <v>2981</v>
       </c>
     </row>
-    <row r="364" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>3103</v>
       </c>
@@ -62016,7 +62052,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="365" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>3104</v>
       </c>
@@ -62024,7 +62060,7 @@
         <v>2983</v>
       </c>
     </row>
-    <row r="366" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>3105</v>
       </c>
@@ -62032,7 +62068,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="367" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>3106</v>
       </c>
@@ -62040,7 +62076,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="368" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>3107</v>
       </c>
@@ -62048,7 +62084,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="369" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>3108</v>
       </c>
@@ -62056,7 +62092,7 @@
         <v>2986</v>
       </c>
     </row>
-    <row r="370" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>3109</v>
       </c>
@@ -62064,7 +62100,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="371" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>37</v>
       </c>
@@ -62188,8 +62224,11 @@
       <c r="AMM371" s="2" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="372" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS371" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>8</v>
       </c>
@@ -62239,7 +62278,7 @@
         <v>4868</v>
       </c>
       <c r="QI372" s="2" t="s">
-        <v>5478</v>
+        <v>5477</v>
       </c>
       <c r="RX372" s="9"/>
       <c r="RY372" s="9" t="s">
@@ -62483,8 +62522,11 @@
       <c r="AMC372" s="2" t="s">
         <v>5392</v>
       </c>
-    </row>
-    <row r="373" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS372" s="2" t="s">
+        <v>5491</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>207</v>
       </c>
@@ -62515,7 +62557,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="374" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>9</v>
       </c>
@@ -62753,13 +62795,16 @@
       <c r="AMC374" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="375" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS374" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>3825</v>
       </c>
     </row>
-    <row r="376" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>10</v>
       </c>
@@ -63065,8 +63110,11 @@
       <c r="AMM376" s="2" t="s">
         <v>4486</v>
       </c>
-    </row>
-    <row r="377" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS376" s="2" t="s">
+        <v>5489</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>3634</v>
       </c>
@@ -63074,7 +63122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>208</v>
       </c>
@@ -63327,7 +63375,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="379" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>11</v>
       </c>
@@ -63569,7 +63617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>12</v>
       </c>
@@ -63613,7 +63661,7 @@
         <v>4866</v>
       </c>
       <c r="QI380" s="2" t="s">
-        <v>5479</v>
+        <v>5478</v>
       </c>
       <c r="RX380" s="9"/>
       <c r="RY380" s="9" t="s">
@@ -63834,12 +63882,12 @@
         <v>4452</v>
       </c>
     </row>
-    <row r="381" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="382" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>530</v>
       </c>
@@ -63853,12 +63901,12 @@
         <v>4228</v>
       </c>
     </row>
-    <row r="383" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="384" spans="1:1027" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>532</v>
       </c>
@@ -63872,12 +63920,12 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="385" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="386" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>534</v>
       </c>
@@ -63891,12 +63939,12 @@
         <v>4453</v>
       </c>
     </row>
-    <row r="387" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="388" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>536</v>
       </c>
@@ -63904,12 +63952,12 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="389" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="390" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>538</v>
       </c>
@@ -63917,12 +63965,12 @@
         <v>4230</v>
       </c>
     </row>
-    <row r="391" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>4260</v>
       </c>
     </row>
-    <row r="392" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>4261</v>
       </c>
@@ -63930,7 +63978,7 @@
         <v>4231</v>
       </c>
     </row>
-    <row r="393" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>94</v>
       </c>
@@ -64042,8 +64090,11 @@
       <c r="AMC393" s="2" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="394" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AMS393" s="2" t="s">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>5324</v>
       </c>
@@ -64090,7 +64141,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="395" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>209</v>
       </c>
@@ -64191,7 +64242,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="396" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>51</v>
       </c>
@@ -64289,7 +64340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>52</v>
       </c>
@@ -64390,7 +64441,7 @@
         <v>4221</v>
       </c>
     </row>
-    <row r="398" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>53</v>
       </c>
@@ -64422,7 +64473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="399" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>54</v>
       </c>
@@ -64517,7 +64568,7 @@
         <v>4221</v>
       </c>
     </row>
-    <row r="400" spans="1:1017" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1017 1033:1033" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>5171</v>
       </c>
@@ -72110,139 +72161,139 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="MR43">
-    <cfRule type="duplicateValues" dxfId="45" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MT43">
-    <cfRule type="duplicateValues" dxfId="44" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MV43">
-    <cfRule type="duplicateValues" dxfId="43" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MX43">
-    <cfRule type="duplicateValues" dxfId="42" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MZ43">
-    <cfRule type="duplicateValues" dxfId="41" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NB43">
-    <cfRule type="duplicateValues" dxfId="40" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ND43">
-    <cfRule type="duplicateValues" dxfId="39" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NF43">
-    <cfRule type="duplicateValues" dxfId="38" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NH43">
-    <cfRule type="duplicateValues" dxfId="37" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NN43">
-    <cfRule type="duplicateValues" dxfId="36" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NP43">
-    <cfRule type="duplicateValues" dxfId="35" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NR43">
-    <cfRule type="duplicateValues" dxfId="34" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NT43">
-    <cfRule type="duplicateValues" dxfId="33" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NV43">
-    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NX43">
-    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NZ43">
-    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OB43">
-    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OD43">
-    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OF43">
-    <cfRule type="duplicateValues" dxfId="27" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OO43">
-    <cfRule type="duplicateValues" dxfId="26" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OP43">
-    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OQ43">
-    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OS1">
-    <cfRule type="duplicateValues" dxfId="23" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="OG1:OH1">
-    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="NI1:NJ1">
-    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="PC1">
-    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="PG1">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKV1 PF1 OT1:PB1 OI1:OR1 NK1:OF1 A1:NH1 QE1:AIN1 AKY1:ALE1 ALM1:ALT1 AMB1:AME1 AMH1:XFD1 AIX1:AKS1">
-    <cfRule type="duplicateValues" dxfId="18" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="PD1:PE1">
-    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="PH1:QD1">
-    <cfRule type="duplicateValues" dxfId="16" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKT1">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKU1">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKT43">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKU43">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKW43">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKW1">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKX43">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AKX1">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ALF1:ALL1">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ALU1:AMA1">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AMF1">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AMG1">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AMF43">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AMG43">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AIO1:AIW1">
-    <cfRule type="duplicateValues" dxfId="1" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="126"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>